<commit_message>
Charges table integrated to app load.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\resources\db\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE96FFF-44D4-4261-8ED9-AF85A609FD92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -651,30 +645,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="15.38671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.38671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.38671875" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -708,7 +702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -725,7 +719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -739,7 +733,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -756,7 +750,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -770,7 +764,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -784,7 +778,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -798,7 +792,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -812,7 +806,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -829,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -843,7 +837,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -860,7 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -874,7 +868,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -888,7 +882,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -902,7 +896,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -916,7 +910,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -930,7 +924,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -944,7 +938,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -958,7 +952,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -972,7 +966,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -989,7 +983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1006,7 +1000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -1020,7 +1014,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1034,7 +1028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1048,7 +1042,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1062,7 +1056,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1076,7 +1070,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1084,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1098,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1112,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1129,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1143,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1157,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1181,7 +1175,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
+  <sortState ref="A2:D35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 3 versions of Criminal Mischief to charges.xlsx check with JH.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BBE2FF-B95C-407E-AC25-6755EAF68CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2993730-A57C-424A-8316-15B7FC8A3333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -283,6 +283,27 @@
   </si>
   <si>
     <t>4511.194</t>
+  </si>
+  <si>
+    <t>Criminal Mischief - Victim is Family or Household Member</t>
+  </si>
+  <si>
+    <t>Criminal Mischief M3</t>
+  </si>
+  <si>
+    <t>2909.07</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Criminal Mischief - Risk of Physical Harm</t>
+  </si>
+  <si>
+    <t>2909.07*</t>
+  </si>
+  <si>
+    <t>2909.07**</t>
   </si>
 </sst>
 </file>
@@ -665,22 +686,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="80.4375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.375" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -714,7 +735,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -731,130 +752,127 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>87</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>68</v>
       </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
@@ -862,58 +880,61 @@
       <c r="D12" t="s">
         <v>82</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B16" s="5">
         <v>4513.04</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>67</v>
@@ -922,286 +943,328 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B28" s="5">
         <v>4511.21</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>68</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>83</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E38" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D39">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Charges to add DOC - persistent.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Admin\Information_Technology\MuniEntry_Files\MuniEntry_app\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8881B31A-D2E5-4EFE-ADA7-14D8D049F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37580C51-93CD-4363-8DFA-80A47690B3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>UCM</t>
+  </si>
+  <si>
+    <t>Disorderly Conduct - Persistent</t>
+  </si>
+  <si>
+    <t>2917.11(A)(1)</t>
+  </si>
+  <si>
+    <t>M4</t>
   </si>
 </sst>
 </file>
@@ -686,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -810,44 +819,44 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
         <v>80</v>
@@ -855,13 +864,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
         <v>80</v>
@@ -869,55 +878,55 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>92</v>
       </c>
-      <c r="D12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -925,44 +934,44 @@
       <c r="D15" t="s">
         <v>80</v>
       </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4513.04</v>
+        <v>67</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -973,41 +982,41 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>80</v>
@@ -1015,13 +1024,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>80</v>
@@ -1029,24 +1038,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>91</v>
@@ -1057,27 +1066,24 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>92</v>
@@ -1086,29 +1092,32 @@
         <v>81</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="5">
-        <v>4511.21</v>
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>91</v>
@@ -1119,10 +1128,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C29" t="s">
         <v>91</v>
@@ -1133,10 +1142,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -1147,10 +1156,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -1161,38 +1170,38 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
@@ -1203,68 +1212,82 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
       </c>
       <c r="D35" t="s">
         <v>80</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
         <v>81</v>
       </c>
-      <c r="E38" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D39">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add charge load to blank working.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Admin\Information_Technology\MuniEntry_Files\MuniEntry_app\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37580C51-93CD-4363-8DFA-80A47690B3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FDB8DC-8320-4166-9B82-9C6FAAC571A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,13 +695,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
@@ -710,7 +710,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,217 +730,210 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
         <v>81</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>92</v>
       </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>92</v>
@@ -948,128 +941,128 @@
       <c r="D16" t="s">
         <v>80</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B18" s="5">
         <v>4513.04</v>
       </c>
-      <c r="C17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C21" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>92</v>
       </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>66</v>
       </c>
-      <c r="D23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>91</v>
@@ -1078,29 +1071,26 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>92</v>
@@ -1109,185 +1099,202 @@
         <v>81</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B30" s="5">
         <v>4511.21</v>
       </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C36" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D39" t="s">
         <v>81</v>
       </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D41">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactoring to single create, open, close db connection functions.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FDB8DC-8320-4166-9B82-9C6FAAC571A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B211EB2-659F-4B2C-A78C-1B55CEB18B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -695,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -753,44 +753,44 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -798,13 +798,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
@@ -812,13 +812,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
@@ -826,13 +826,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>76</v>
@@ -840,44 +840,44 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
         <v>80</v>
@@ -885,13 +885,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
         <v>80</v>
@@ -899,55 +899,55 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A15" s="4" t="s">
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -955,44 +955,44 @@
       <c r="D17" t="s">
         <v>80</v>
       </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="5">
-        <v>4513.04</v>
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
@@ -1003,41 +1003,41 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -1045,13 +1045,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
         <v>80</v>
@@ -1059,24 +1059,24 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
@@ -1087,27 +1087,24 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>92</v>
@@ -1116,29 +1113,32 @@
         <v>81</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5">
-        <v>4511.21</v>
+        <v>78</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="B31" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -1191,38 +1191,38 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -1233,68 +1233,82 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
         <v>80</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
         <v>80</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
         <v>81</v>
       </c>
-      <c r="E40" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D42">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continued refactoring - passing.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B211EB2-659F-4B2C-A78C-1B55CEB18B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13134389-8FE3-4CFC-8EC2-43FED29AAA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>M4</t>
+  </si>
+  <si>
+    <t>AaTest</t>
+  </si>
+  <si>
+    <t>1111.11</t>
+  </si>
+  <si>
+    <t>BBTest</t>
+  </si>
+  <si>
+    <t>1222.22</t>
   </si>
 </sst>
 </file>
@@ -695,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -738,84 +750,86 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>80</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>87</v>
@@ -826,13 +840,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>88</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>76</v>
@@ -840,13 +854,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
         <v>76</v>
@@ -854,58 +868,58 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>63</v>
+        <v>93</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
         <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
@@ -913,10 +927,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -926,28 +940,25 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
+      <c r="A16" t="s">
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -957,84 +968,87 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>54</v>
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4513.04</v>
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>67</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
         <v>80</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>11</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>91</v>
@@ -1045,27 +1059,27 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
         <v>80</v>
@@ -1073,100 +1087,100 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="5">
-        <v>4511.21</v>
+        <v>51</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -1177,10 +1191,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -1191,10 +1205,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
@@ -1205,24 +1219,24 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -1233,41 +1247,38 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
         <v>80</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
         <v>91</v>
@@ -1278,37 +1289,68 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
         <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>92</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>81</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E43" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D44">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Testing db_charges updating - will add but not delete new charges.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13134389-8FE3-4CFC-8EC2-43FED29AAA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D85D46-1ABE-4FAA-A066-54BFC576FE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -313,18 +313,6 @@
   </si>
   <si>
     <t>M4</t>
-  </si>
-  <si>
-    <t>AaTest</t>
-  </si>
-  <si>
-    <t>1111.11</t>
-  </si>
-  <si>
-    <t>BBTest</t>
-  </si>
-  <si>
-    <t>1222.22</t>
   </si>
 </sst>
 </file>
@@ -707,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -750,86 +738,84 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>87</v>
@@ -840,13 +826,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>76</v>
@@ -854,13 +840,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
         <v>76</v>
@@ -868,58 +854,58 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>62</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
         <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
@@ -927,10 +913,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>79</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -940,25 +926,28 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>64</v>
+      <c r="A16" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -968,87 +957,84 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5">
-        <v>4513.04</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>91</v>
@@ -1059,27 +1045,27 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>80</v>
@@ -1087,100 +1073,100 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>78</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="B31" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>25</v>
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -1191,10 +1177,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="5">
-        <v>4511.21</v>
+        <v>70</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -1205,10 +1191,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
@@ -1219,24 +1205,24 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -1247,38 +1233,41 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
         <v>80</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>91</v>
@@ -1289,68 +1278,37 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="E41" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D42">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored charges tables creation - working.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D85D46-1ABE-4FAA-A066-54BFC576FE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A715E3-96F4-4765-A1EC-115E1CA624E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -731,11 +731,18 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -753,44 +760,44 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -798,13 +805,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
@@ -812,13 +819,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>90</v>
+        <v>41</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
@@ -826,13 +833,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
         <v>76</v>
@@ -840,44 +847,44 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>80</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
         <v>80</v>
@@ -885,13 +892,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>80</v>
@@ -899,55 +906,55 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
-        <v>79</v>
+      <c r="A15" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
         <v>92</v>
       </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>91</v>
-      </c>
       <c r="D16" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -955,44 +962,44 @@
       <c r="D17" t="s">
         <v>80</v>
       </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4513.04</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
@@ -1003,41 +1010,41 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -1045,13 +1052,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>80</v>
@@ -1059,24 +1066,24 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
@@ -1087,24 +1094,27 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>92</v>
@@ -1113,32 +1123,29 @@
         <v>81</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>78</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -1149,10 +1156,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="5">
-        <v>4511.21</v>
+        <v>57</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -1163,10 +1170,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -1177,10 +1184,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -1191,38 +1198,38 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -1233,82 +1240,68 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
         <v>80</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
         <v>80</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="E40" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 6 OVI charges to charges 1-3 for 4511.19 A1 and A2.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A715E3-96F4-4765-A1EC-115E1CA624E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB44ED70-62C5-4C2E-A4EB-9274EC201E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -313,6 +313,42 @@
   </si>
   <si>
     <t>M4</t>
+  </si>
+  <si>
+    <t>OVI Alcohol / Drugs 1st</t>
+  </si>
+  <si>
+    <t>OVI Alcohol / Drugs 2nd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OVI Alcohol / Drugs 3rd </t>
+  </si>
+  <si>
+    <t>4511.19(A)(1)*</t>
+  </si>
+  <si>
+    <t>4511.19(A)(1)**</t>
+  </si>
+  <si>
+    <t>4511.19(A)(1)***</t>
+  </si>
+  <si>
+    <t>OVI Refusal 1st / Prior in Past 20 Years</t>
+  </si>
+  <si>
+    <t>OVI Refusal 2nd / Prior in Past 20 Years</t>
+  </si>
+  <si>
+    <t>OVI Refusal 3rd / Prior in Past 20 Years</t>
+  </si>
+  <si>
+    <t>4511.19(A)(2)*</t>
+  </si>
+  <si>
+    <t>4511.19(A)(2)**</t>
+  </si>
+  <si>
+    <t>4511.19(A)(2)***</t>
   </si>
 </sst>
 </file>
@@ -695,16 +731,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5625" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.375" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
@@ -1052,10 +1088,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>66</v>
@@ -1066,75 +1102,69 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>43</v>
+        <v>98</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>102</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>103</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
         <v>80</v>
@@ -1142,13 +1172,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5">
-        <v>4511.21</v>
+        <v>82</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>80</v>
@@ -1156,66 +1186,72 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
         <v>81</v>
       </c>
+      <c r="E34" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>78</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -1226,10 +1262,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="B36" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -1240,27 +1276,24 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
         <v>80</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
@@ -1271,37 +1304,124 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
         <v>81</v>
       </c>
-      <c r="E40" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored main_window, database sql load and added attorney xlsx.
Set case to load clean and working.


Refactored CriminalCaseInfo in SqlRetriever to CmsCaseInfo


Mypy passing on main_window


Renaming variables in main_window


Refactored show hide case lists.


Mypy passing and pylint at 9.4.


Added Attorney Excel file to load attorneys.


Added attorneys to list and it is working.


Test passing.
</commit_message>
<xml_diff>
--- a/db/Charges.xlsx
+++ b/db/Charges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Admin\Information_Technology\MuniEntry_Files\MuniEntry_app\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D215D0-F173-4777-AE65-47272ED1DCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37847CDF-8219-4847-B016-80D05137D029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -739,11 +739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.625" style="3" customWidth="1"/>
@@ -752,7 +752,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -786,7 +786,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -800,7 +800,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -817,7 +817,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -831,7 +831,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -845,7 +845,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -859,7 +859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -873,7 +873,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -887,7 +887,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -904,7 +904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -918,7 +918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -932,7 +932,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -946,7 +946,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -960,7 +960,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
@@ -977,7 +977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -991,7 +991,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>108</v>
       </c>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>16</v>
       </c>

</xml_diff>